<commit_message>
Adding node_modules manually because of missing python
</commit_message>
<xml_diff>
--- a/target.xlsx
+++ b/target.xlsx
@@ -5,21 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramez\Desktop\Stubs Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RamezA\Desktop\Stubs Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9324"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5784"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="79">
   <si>
     <t>Service URL</t>
   </si>
@@ -240,22 +240,28 @@
     <t>Paul.Bew112</t>
   </si>
   <si>
-    <t>GEO123</t>
-  </si>
-  <si>
-    <t>demo.Sunday</t>
-  </si>
-  <si>
-    <t>49152820712345</t>
-  </si>
-  <si>
     <t>CDEV12</t>
+  </si>
+  <si>
+    <t>Kickoff</t>
+  </si>
+  <si>
+    <t>Mona</t>
+  </si>
+  <si>
+    <t>MaiAbdelFatah</t>
+  </si>
+  <si>
+    <t>48917777777777</t>
+  </si>
+  <si>
+    <t>Mai124</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
@@ -877,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -927,7 +933,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="12" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>70</v>
@@ -1067,7 +1073,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="12" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>67</v>
@@ -1273,7 +1279,7 @@
         <v>47</v>
       </c>
       <c r="E19" s="35" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="F19" s="35" t="s">
         <v>39</v>
@@ -1351,7 +1357,7 @@
         <v>50</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F22" s="35" t="s">
         <v>42</v>
@@ -1403,7 +1409,7 @@
         <v>52</v>
       </c>
       <c r="E24" s="18">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F24" s="18">
         <v>3</v>
@@ -1429,7 +1435,7 @@
         <v>53</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F25" s="35" t="s">
         <v>43</v>
@@ -1507,7 +1513,7 @@
         <v>56</v>
       </c>
       <c r="E28" s="35" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="F28" s="35" t="s">
         <v>44</v>
@@ -1559,7 +1565,7 @@
         <v>58</v>
       </c>
       <c r="E30" s="18">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F30" s="18">
         <v>3</v>
@@ -1666,5 +1672,8 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;7&amp;K000000C2 General</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>